<commit_message>
Update Kế hoạch dự án theo Agile - nhóm 10.xlsx
</commit_message>
<xml_diff>
--- a/docs/01 - Tai lieu du an/Kế hoạch dự án theo Agile - nhóm 10.xlsx
+++ b/docs/01 - Tai lieu du an/Kế hoạch dự án theo Agile - nhóm 10.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Group-10-156724-Software-Engineering\docs\01 - Tai lieu du an\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\Group-10-156724-Software-Engineering\docs\01 - Tai lieu du an\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F85E94-A16E-4C32-83B8-ECB0D1877FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F6E1C8-A897-4ED6-B4A7-FC77452E6BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,15 +49,6 @@
   </si>
   <si>
     <t>Phần mềm quản lý chung cư</t>
-  </si>
-  <si>
-    <t>Nguyễn Khắc Tiếp</t>
-  </si>
-  <si>
-    <t>3-tháng 12-2023</t>
-  </si>
-  <si>
-    <t>5-tháng 2-2024</t>
   </si>
   <si>
     <t>SCOPE STATEMENT</t>
@@ -252,6 +243,15 @@
   <si>
     <t xml:space="preserve">Nguyễn Mạnh Thái Hà
 </t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Thành Đạt</t>
+  </si>
+  <si>
+    <t>1-tháng 5-2025</t>
+  </si>
+  <si>
+    <t>5-tháng 7-2025</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="4472C4"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -621,76 +621,76 @@
                 <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>45263</c:v>
+                  <c:v>45778</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45263</c:v>
+                  <c:v>45778</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45263</c:v>
+                  <c:v>45778</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45263</c:v>
+                  <c:v>45778</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45263</c:v>
+                  <c:v>45778</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45274</c:v>
+                  <c:v>45789</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45274</c:v>
+                  <c:v>45789</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45274</c:v>
+                  <c:v>45789</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45274</c:v>
+                  <c:v>45789</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45281</c:v>
+                  <c:v>45796</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45281</c:v>
+                  <c:v>45796</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45285</c:v>
+                  <c:v>45800</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45296</c:v>
+                  <c:v>45811</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45300</c:v>
+                  <c:v>45815</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45300</c:v>
+                  <c:v>45815</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>45300</c:v>
+                  <c:v>45815</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>45301</c:v>
+                  <c:v>45816</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>45303</c:v>
+                  <c:v>45818</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>45303</c:v>
+                  <c:v>45818</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>45303</c:v>
+                  <c:v>45818</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>45303</c:v>
+                  <c:v>45818</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>45306</c:v>
+                  <c:v>45821</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>45306</c:v>
+                  <c:v>45821</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>45325</c:v>
+                  <c:v>45839</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -723,7 +723,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="ED7D31"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1285,9 +1285,9 @@
   </sheetPr>
   <dimension ref="A1:AE1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1392,13 +1392,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="11">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="1"/>
@@ -1466,34 +1466,34 @@
     <row r="5" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="H5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="I5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="J5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>21</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -1520,24 +1520,24 @@
       <c r="A6" s="1"/>
       <c r="B6" s="13"/>
       <c r="C6" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="15">
-        <v>45263</v>
+        <v>45778</v>
       </c>
       <c r="H6" s="15">
-        <v>45272</v>
+        <v>45787</v>
       </c>
       <c r="I6" s="14">
         <v>9</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K6" s="14"/>
       <c r="L6" s="3"/>
@@ -1565,31 +1565,31 @@
       <c r="A7" s="1"/>
       <c r="B7" s="16"/>
       <c r="C7" s="17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F7" s="17">
         <v>5</v>
       </c>
       <c r="G7" s="15">
-        <v>45263</v>
+        <v>45778</v>
       </c>
       <c r="H7" s="18">
-        <v>45265</v>
+        <v>45780</v>
       </c>
       <c r="I7" s="17">
         <v>2</v>
       </c>
       <c r="J7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>23</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>26</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -1616,31 +1616,31 @@
       <c r="A8" s="1"/>
       <c r="B8" s="16"/>
       <c r="C8" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F8" s="17">
         <v>7</v>
       </c>
       <c r="G8" s="15">
-        <v>45263</v>
+        <v>45778</v>
       </c>
       <c r="H8" s="18">
-        <v>45268</v>
+        <v>45781</v>
       </c>
       <c r="I8" s="17">
         <v>3</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1667,31 +1667,31 @@
       <c r="A9" s="1"/>
       <c r="B9" s="16"/>
       <c r="C9" s="17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F9" s="17">
         <v>6</v>
       </c>
       <c r="G9" s="15">
-        <v>45263</v>
+        <v>45778</v>
       </c>
       <c r="H9" s="18">
-        <v>45270</v>
+        <v>45783</v>
       </c>
       <c r="I9" s="17">
         <v>5</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -1718,31 +1718,31 @@
       <c r="A10" s="1"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F10" s="17">
         <v>6</v>
       </c>
       <c r="G10" s="15">
-        <v>45263</v>
+        <v>45778</v>
       </c>
       <c r="H10" s="18">
-        <v>45272</v>
+        <v>45782</v>
       </c>
       <c r="I10" s="17">
         <v>4</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L10" s="17"/>
       <c r="M10" s="3"/>
@@ -1769,24 +1769,24 @@
       <c r="A11" s="1"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21">
-        <v>45274</v>
+        <v>45789</v>
       </c>
       <c r="H11" s="22">
-        <v>45280</v>
+        <v>45795</v>
       </c>
       <c r="I11" s="20">
         <v>6</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K11" s="20"/>
       <c r="L11" s="3"/>
@@ -1814,31 +1814,31 @@
       <c r="A12" s="1"/>
       <c r="B12" s="16"/>
       <c r="C12" s="23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F12" s="23">
         <v>6</v>
       </c>
       <c r="G12" s="21">
-        <v>45274</v>
+        <v>45789</v>
       </c>
       <c r="H12" s="22">
-        <v>45280</v>
+        <v>45795</v>
       </c>
       <c r="I12" s="23">
         <v>6</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K12" s="23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1865,31 +1865,31 @@
       <c r="A13" s="1"/>
       <c r="B13" s="16"/>
       <c r="C13" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F13" s="23">
         <v>8</v>
       </c>
       <c r="G13" s="21">
-        <v>45274</v>
+        <v>45789</v>
       </c>
       <c r="H13" s="22">
-        <v>45278</v>
+        <v>45793</v>
       </c>
       <c r="I13" s="23">
         <v>4</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K13" s="23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -1916,31 +1916,31 @@
       <c r="A14" s="1"/>
       <c r="B14" s="16"/>
       <c r="C14" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F14" s="23">
         <v>8</v>
       </c>
       <c r="G14" s="21">
-        <v>45274</v>
+        <v>45789</v>
       </c>
       <c r="H14" s="22">
-        <v>45280</v>
+        <v>45793</v>
       </c>
       <c r="I14" s="23">
         <v>4</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K14" s="23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -1967,24 +1967,24 @@
       <c r="A15" s="1"/>
       <c r="B15" s="16"/>
       <c r="C15" s="24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F15" s="24"/>
       <c r="G15" s="25">
-        <v>45281</v>
+        <v>45796</v>
       </c>
       <c r="H15" s="22">
-        <v>45299</v>
+        <v>45814</v>
       </c>
       <c r="I15" s="24">
         <v>18</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K15" s="24"/>
       <c r="L15" s="3"/>
@@ -2012,31 +2012,31 @@
       <c r="A16" s="1"/>
       <c r="B16" s="16"/>
       <c r="C16" s="23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F16" s="23">
         <v>10</v>
       </c>
       <c r="G16" s="25">
-        <v>45281</v>
+        <v>45796</v>
       </c>
       <c r="H16" s="22">
-        <v>45292</v>
+        <v>45807</v>
       </c>
       <c r="I16" s="23">
         <v>11</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K16" s="23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -2063,31 +2063,31 @@
       <c r="A17" s="1"/>
       <c r="B17" s="16"/>
       <c r="C17" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F17" s="23">
         <v>7</v>
       </c>
       <c r="G17" s="25">
-        <v>45285</v>
+        <v>45800</v>
       </c>
       <c r="H17" s="22">
-        <v>45296</v>
+        <v>45811</v>
       </c>
       <c r="I17" s="23">
         <v>11</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -2114,31 +2114,31 @@
       <c r="A18" s="1"/>
       <c r="B18" s="16"/>
       <c r="C18" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F18" s="23">
         <v>8</v>
       </c>
       <c r="G18" s="25">
-        <v>45296</v>
+        <v>45811</v>
       </c>
       <c r="H18" s="22">
-        <v>45299</v>
+        <v>45814</v>
       </c>
       <c r="I18" s="23">
         <v>3</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -2165,24 +2165,24 @@
       <c r="A19" s="1"/>
       <c r="B19" s="16"/>
       <c r="C19" s="24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F19" s="24"/>
       <c r="G19" s="25">
-        <v>45300</v>
+        <v>45815</v>
       </c>
       <c r="H19" s="22">
-        <v>45303</v>
+        <v>45818</v>
       </c>
       <c r="I19" s="24">
         <v>3</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K19" s="24"/>
       <c r="L19" s="3"/>
@@ -2210,31 +2210,31 @@
       <c r="A20" s="1"/>
       <c r="B20" s="16"/>
       <c r="C20" s="23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F20" s="23">
         <v>5</v>
       </c>
       <c r="G20" s="25">
-        <v>45300</v>
+        <v>45815</v>
       </c>
       <c r="H20" s="22">
-        <v>45302</v>
+        <v>45817</v>
       </c>
       <c r="I20" s="23">
         <v>2</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K20" s="23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -2261,31 +2261,31 @@
       <c r="A21" s="1"/>
       <c r="B21" s="16"/>
       <c r="C21" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F21" s="23">
         <v>7</v>
       </c>
       <c r="G21" s="25">
-        <v>45300</v>
+        <v>45815</v>
       </c>
       <c r="H21" s="22">
-        <v>45301</v>
+        <v>45816</v>
       </c>
       <c r="I21" s="23">
         <v>1</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K21" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -2312,31 +2312,31 @@
       <c r="A22" s="1"/>
       <c r="B22" s="16"/>
       <c r="C22" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F22" s="23">
         <v>5</v>
       </c>
       <c r="G22" s="25">
-        <v>45301</v>
+        <v>45816</v>
       </c>
       <c r="H22" s="22">
-        <v>45627</v>
+        <v>45818</v>
       </c>
       <c r="I22" s="23">
         <v>2</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K22" s="23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -2363,24 +2363,24 @@
       <c r="A23" s="1"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="25">
-        <v>45303</v>
+        <v>45818</v>
       </c>
       <c r="H23" s="22">
-        <v>45305</v>
+        <v>45820</v>
       </c>
       <c r="I23" s="24">
         <v>2</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K23" s="24"/>
       <c r="L23" s="3"/>
@@ -2408,31 +2408,31 @@
       <c r="A24" s="1"/>
       <c r="B24" s="16"/>
       <c r="C24" s="23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F24" s="23">
         <v>8</v>
       </c>
       <c r="G24" s="25">
-        <v>45303</v>
+        <v>45818</v>
       </c>
       <c r="H24" s="22">
-        <v>45305</v>
+        <v>45820</v>
       </c>
       <c r="I24" s="23">
         <v>2</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K24" s="23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -2459,31 +2459,31 @@
       <c r="A25" s="1"/>
       <c r="B25" s="16"/>
       <c r="C25" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F25" s="23">
         <v>3</v>
       </c>
       <c r="G25" s="25">
-        <v>45303</v>
+        <v>45818</v>
       </c>
       <c r="H25" s="22">
-        <v>45305</v>
+        <v>45820</v>
       </c>
       <c r="I25" s="23">
         <v>2</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K25" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2510,24 +2510,24 @@
       <c r="A26" s="1"/>
       <c r="B26" s="24"/>
       <c r="C26" s="24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" s="26"/>
       <c r="E26" s="26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="25">
-        <v>45303</v>
+        <v>45818</v>
       </c>
       <c r="H26" s="22">
-        <v>45305</v>
+        <v>45820</v>
       </c>
       <c r="I26" s="24">
         <v>2</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K26" s="24"/>
       <c r="L26" s="3"/>
@@ -2545,31 +2545,31 @@
       <c r="A27" s="1"/>
       <c r="B27" s="16"/>
       <c r="C27" s="23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F27" s="23">
         <v>10</v>
       </c>
       <c r="G27" s="25">
-        <v>45306</v>
+        <v>45821</v>
       </c>
       <c r="H27" s="22">
-        <v>45325</v>
+        <v>45839</v>
       </c>
       <c r="I27" s="23">
         <v>19</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K27" s="23" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -2596,31 +2596,31 @@
       <c r="A28" s="1"/>
       <c r="B28" s="16"/>
       <c r="C28" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F28" s="23">
         <v>10</v>
       </c>
       <c r="G28" s="25">
-        <v>45306</v>
+        <v>45821</v>
       </c>
       <c r="H28" s="22">
-        <v>45323</v>
+        <v>45838</v>
       </c>
       <c r="I28" s="23">
         <v>17</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K28" s="23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -2647,31 +2647,31 @@
       <c r="A29" s="1"/>
       <c r="B29" s="16"/>
       <c r="C29" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F29" s="23">
         <v>10</v>
       </c>
       <c r="G29" s="25">
-        <v>45325</v>
+        <v>45839</v>
       </c>
       <c r="H29" s="22">
-        <v>45327</v>
+        <v>45842</v>
       </c>
       <c r="I29" s="23">
         <v>3</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K29" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>

</xml_diff>